<commit_message>
updated game design document
</commit_message>
<xml_diff>
--- a/game_design/TreeWars_balancing.xlsx
+++ b/game_design/TreeWars_balancing.xlsx
@@ -4,19 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="14370"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="14370" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tree" sheetId="1" r:id="rId1"/>
+    <sheet name="Environment" sheetId="2" r:id="rId2"/>
+    <sheet name="Mechanics" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="divider">Tree!$B$76</definedName>
+    <definedName name="exponent">Tree!$B$77</definedName>
+    <definedName name="Light_units_generated_standard">Tree!$B$47</definedName>
+    <definedName name="Set_foilage_density">Tree!$D$67</definedName>
+    <definedName name="Set_light_input">Tree!$F$67</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="143">
   <si>
     <t>Basics</t>
   </si>
@@ -120,12 +127,6 @@
     <t>Light units required by tree top size</t>
   </si>
   <si>
-    <t>Free light units by width (foilage density = 5)</t>
-  </si>
-  <si>
-    <t>Free light units by width (foilage density = 3)</t>
-  </si>
-  <si>
     <t>Tree top size by width and height</t>
   </si>
   <si>
@@ -133,6 +134,324 @@
   </si>
   <si>
     <t>exponent:</t>
+  </si>
+  <si>
+    <t>Set foilage density:</t>
+  </si>
+  <si>
+    <t>Free light units by width</t>
+  </si>
+  <si>
+    <t>Set light input:</t>
+  </si>
+  <si>
+    <t>Weather Effects</t>
+  </si>
+  <si>
+    <t>Weather effects length (seconds):</t>
+  </si>
+  <si>
+    <t>Effect name:</t>
+  </si>
+  <si>
+    <t>Sunshine</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>Effect1:</t>
+  </si>
+  <si>
+    <t>Effect2:</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Adds 2 points of light input</t>
+  </si>
+  <si>
+    <t>Increases synthesis rate by 25% points</t>
+  </si>
+  <si>
+    <t>Adds +5% points soil moisture</t>
+  </si>
+  <si>
+    <t>Hazard name:</t>
+  </si>
+  <si>
+    <t>Cold spell</t>
+  </si>
+  <si>
+    <t>Reduces foilage density by 1 level</t>
+  </si>
+  <si>
+    <t>Drought</t>
+  </si>
+  <si>
+    <t>Reduces soil moisture by 20% points</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>5% chance for each height level above minimum height to break off</t>
+  </si>
+  <si>
+    <t>(tree top size/(root areas*root strength)) % chance to uproot and kill tree</t>
+  </si>
+  <si>
+    <t>Reduces water pool by 20%</t>
+  </si>
+  <si>
+    <t>Cancels out with Sunshine</t>
+  </si>
+  <si>
+    <t>Cancels out with Rain</t>
+  </si>
+  <si>
+    <t>Ends Spring</t>
+  </si>
+  <si>
+    <t>10% chance of gaining a bonus feature</t>
+  </si>
+  <si>
+    <t>Bonus Features</t>
+  </si>
+  <si>
+    <t>Feature name:</t>
+  </si>
+  <si>
+    <t>Symbiotic Fungus Colony</t>
+  </si>
+  <si>
+    <t>Adds 10% synthesis output</t>
+  </si>
+  <si>
+    <t>Bird Nest</t>
+  </si>
+  <si>
+    <t>Adds 1 weather effect point per 10 s</t>
+  </si>
+  <si>
+    <t>Nutrient Synthesis rule</t>
+  </si>
+  <si>
+    <t>Nutrient Synthesis</t>
+  </si>
+  <si>
+    <t>(light_level/water_level)^(SIGN(light_level-water_level))</t>
+  </si>
+  <si>
+    <t>Root Areas</t>
+  </si>
+  <si>
+    <t>Water intake</t>
+  </si>
+  <si>
+    <t>soil humidity</t>
+  </si>
+  <si>
+    <t>root branching level</t>
+  </si>
+  <si>
+    <t>Tree top size water requirement</t>
+  </si>
+  <si>
+    <t>(size*3)</t>
+  </si>
+  <si>
+    <t>Water generated:</t>
+  </si>
+  <si>
+    <t>humidity intake per second (%):</t>
+  </si>
+  <si>
+    <t>soil_humidity*humidity_intake/8</t>
+  </si>
+  <si>
+    <t>Mechanic description</t>
+  </si>
+  <si>
+    <t>Trees take in Water through the Roots</t>
+  </si>
+  <si>
+    <t>Roots grow in the Soil hexes</t>
+  </si>
+  <si>
+    <t>Roots can grow into an enemy soil hex if their Strength is at least equal to the enemy root's Strength</t>
+  </si>
+  <si>
+    <t>A high Root Strength decreases risk of uprooting in a Storm</t>
+  </si>
+  <si>
+    <t>The Branching level indicates how much Soil Humidity a root converts into Water every second</t>
+  </si>
+  <si>
+    <t>A soil hex's soil humidity is reduced when a root converts humidity into water</t>
+  </si>
+  <si>
+    <t>Roots can grow into any free hex adjacent to an already existing root</t>
+  </si>
+  <si>
+    <t>Every horizontal segment has a Light input</t>
+  </si>
+  <si>
+    <t>Trees take in Water and Energy to generate Nutrients</t>
+  </si>
+  <si>
+    <t>Trees convert Light input into Energy through their Foilage</t>
+  </si>
+  <si>
+    <t>Trees take in Light for every horizontal segment their Treetop occupies</t>
+  </si>
+  <si>
+    <t>Treetop growth is not limited in Height</t>
+  </si>
+  <si>
+    <t>A treetop's Width can never grow greater than twice its Height</t>
+  </si>
+  <si>
+    <t>When growing in width, treetops always grow one space on BOTH sides</t>
+  </si>
+  <si>
+    <t>When growing in width, treetops can overlap with other treetops</t>
+  </si>
+  <si>
+    <t>If two or more treetops overlap, the tree with the greater Height converts first, only then is the remaining light converted by the next higher tree</t>
+  </si>
+  <si>
+    <t>If two or more trees have the same height, they share Light input evenly</t>
+  </si>
+  <si>
+    <t>A treetop's area determines how much Water and Energy the tree requires to sustain itself every second</t>
+  </si>
+  <si>
+    <t>Water and Energy are first taken from the intake</t>
+  </si>
+  <si>
+    <t>If an intake is not sufficient to sustain the tree, the tree takes the resource from its Reserves</t>
+  </si>
+  <si>
+    <t>Any Water and Energy left over after sustaining the tree is partially converted into Nutrients, the rest is stored in the tree's Reserves</t>
+  </si>
+  <si>
+    <t>A tree tries to convert 50% of the greater intake into nutrients</t>
+  </si>
+  <si>
+    <t>One unit of Water and one unit of Energy are converted into one unit of Nutrient</t>
+  </si>
+  <si>
+    <t>A tree's roots have a Strength level (1-5)</t>
+  </si>
+  <si>
+    <t>A tree's roots have a Branching level (1-5)</t>
+  </si>
+  <si>
+    <t>Treetops can grow in Height (4-10) and Width (3-19)</t>
+  </si>
+  <si>
+    <t>Light input varies by weather (10 or 12)</t>
+  </si>
+  <si>
+    <t>A tree's Foilage has a Density level (0-5)</t>
+  </si>
+  <si>
+    <t>Foilage density determines how much Light input is converted into Energy (34%-100%)</t>
+  </si>
+  <si>
+    <t>Every Soil hex has a soil humidity (0%-100%)</t>
+  </si>
+  <si>
+    <t>If a tree has depleted a Reserve, it takes Damage</t>
+  </si>
+  <si>
+    <t>When a tree takes damage, it converts Health into Nutrients</t>
+  </si>
+  <si>
+    <t>When a tree's Health reaches zero, it is killed (GAME OVER)</t>
+  </si>
+  <si>
+    <t>Missing Water or Energy is taken from the Reserve</t>
+  </si>
+  <si>
+    <t>If a Reserve is depleted, no more Nutrients are generated</t>
+  </si>
+  <si>
+    <t>Nutrients are used to grow all aspects of the tree (see above)</t>
+  </si>
+  <si>
+    <t>A player gains Weather points over time</t>
+  </si>
+  <si>
+    <t>Sunshine increases the Light input to 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather Effects last for 10 seconds or until Canceled </t>
+  </si>
+  <si>
+    <t>Sunshine cancels out Rain</t>
+  </si>
+  <si>
+    <t>Weather points can be used to activate Weather Effects (Sunshine, Rain, Spring)</t>
+  </si>
+  <si>
+    <t>Rain adds +5% points humidity to all soil hexes every second</t>
+  </si>
+  <si>
+    <t>Rain cancels out Sunshine</t>
+  </si>
+  <si>
+    <t>Spring increases maximum Water/Energy conversion to 75%</t>
+  </si>
+  <si>
+    <t>When a player activates a Weather Effect a random enemy player is awarded a Hazard point</t>
+  </si>
+  <si>
+    <t>Hazard points can be spent to to activate Hazards (Cold Snap, Drought, Storm)</t>
+  </si>
+  <si>
+    <t>When two effects cancel out, the new effect's duration is reduced by the current effect's remaining duration</t>
+  </si>
+  <si>
+    <t>Cold Snap</t>
+  </si>
+  <si>
+    <t>A Cold Snap reduces all trees' Foilage density by one (to a minimum of zero)</t>
+  </si>
+  <si>
+    <t>A Cold Snap ends Spring immediately</t>
+  </si>
+  <si>
+    <t>A Drought reduces all soil hexes' humidity by 20% points</t>
+  </si>
+  <si>
+    <t>A Drought reduces all trees' Water Reserves by 20%</t>
+  </si>
+  <si>
+    <t>A Storm has a chance to uproot and kill a tree (GAME OVER)</t>
+  </si>
+  <si>
+    <t>A Storm blows either from left to right or from right to left</t>
+  </si>
+  <si>
+    <t>The chance that a tree is uprooted is (tree top size/(root areas*root strength)) %</t>
+  </si>
+  <si>
+    <t>A Storm "hits" trees in sequence (i.e. a storm blowing from left to right hits the left-most tree first, then the second tree from the left and so on)</t>
+  </si>
+  <si>
+    <t>A Storm has a chance to break off Height from a treetop</t>
+  </si>
+  <si>
+    <t>Heigth levels that are required to support a tree's Width cannot break off</t>
+  </si>
+  <si>
+    <t>Any additional Height levels have a 5% chance to break off</t>
+  </si>
+  <si>
+    <t>This chance is divided by 2 for every tree the sotrm has already hit</t>
   </si>
 </sst>
 </file>
@@ -190,117 +509,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -649,10 +858,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:S79"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,20 +872,23 @@
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -689,8 +901,14 @@
       <c r="E4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -704,7 +922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -712,7 +930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -720,7 +938,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -728,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -737,7 +955,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -746,12 +964,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -762,7 +980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -957,7 +1175,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1343,39 +1561,39 @@
         <v>0</v>
       </c>
       <c r="B50" s="2">
-        <f>$C26/100*$B$47*B$49</f>
+        <f>$C26/100*Light_units_generated_standard*B$49</f>
         <v>10.200000000000001</v>
       </c>
       <c r="C50" s="2">
-        <f t="shared" ref="C50:J50" si="3">$C26/100*$B$47*C$49</f>
+        <f>$C26/100*Light_units_generated_standard*C$49</f>
         <v>17</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" si="3"/>
+        <f>$C26/100*Light_units_generated_standard*D$49</f>
         <v>23.800000000000004</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="3"/>
+        <f>$C26/100*Light_units_generated_standard*E$49</f>
         <v>30.6</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="3"/>
+        <f>$C26/100*Light_units_generated_standard*F$49</f>
         <v>37.400000000000006</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="3"/>
+        <f>$C26/100*Light_units_generated_standard*G$49</f>
         <v>44.2</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="3"/>
+        <f>$C26/100*Light_units_generated_standard*H$49</f>
         <v>51.000000000000007</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="3"/>
+        <f>$C26/100*Light_units_generated_standard*I$49</f>
         <v>57.800000000000004</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="3"/>
+        <f>$C26/100*Light_units_generated_standard*J$49</f>
         <v>64.600000000000009</v>
       </c>
     </row>
@@ -1384,39 +1602,39 @@
         <v>1</v>
       </c>
       <c r="B51" s="2">
-        <f t="shared" ref="B51:J55" si="4">$C27/100*$B$47*B$49</f>
+        <f>$C27/100*Light_units_generated_standard*B$49</f>
         <v>20.400000000000002</v>
       </c>
       <c r="C51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*C$49</f>
         <v>34</v>
       </c>
       <c r="D51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*D$49</f>
         <v>47.600000000000009</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*E$49</f>
         <v>61.2</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*F$49</f>
         <v>74.800000000000011</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*G$49</f>
         <v>88.4</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*H$49</f>
         <v>102.00000000000001</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*I$49</f>
         <v>115.60000000000001</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="4"/>
+        <f>$C27/100*Light_units_generated_standard*J$49</f>
         <v>129.20000000000002</v>
       </c>
     </row>
@@ -1425,39 +1643,39 @@
         <v>2</v>
       </c>
       <c r="B52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*B$49</f>
         <v>22.799999999999997</v>
       </c>
       <c r="C52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*C$49</f>
         <v>38</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*D$49</f>
         <v>53.199999999999996</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*E$49</f>
         <v>68.399999999999991</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*F$49</f>
         <v>83.6</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*G$49</f>
         <v>98.8</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*H$49</f>
         <v>114</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*I$49</f>
         <v>129.19999999999999</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="4"/>
+        <f>$C28/100*Light_units_generated_standard*J$49</f>
         <v>144.4</v>
       </c>
     </row>
@@ -1466,39 +1684,39 @@
         <v>3</v>
       </c>
       <c r="B53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*B$49</f>
         <v>25.200000000000003</v>
       </c>
       <c r="C53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*C$49</f>
         <v>42</v>
       </c>
       <c r="D53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*D$49</f>
         <v>58.800000000000004</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*E$49</f>
         <v>75.600000000000009</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*F$49</f>
         <v>92.4</v>
       </c>
       <c r="G53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*G$49</f>
         <v>109.2</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*H$49</f>
         <v>126</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*I$49</f>
         <v>142.80000000000001</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" si="4"/>
+        <f>$C29/100*Light_units_generated_standard*J$49</f>
         <v>159.6</v>
       </c>
     </row>
@@ -1507,39 +1725,39 @@
         <v>4</v>
       </c>
       <c r="B54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*B$49</f>
         <v>27.6</v>
       </c>
       <c r="C54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*C$49</f>
         <v>46.000000000000007</v>
       </c>
       <c r="D54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*D$49</f>
         <v>64.400000000000006</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*E$49</f>
         <v>82.800000000000011</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*F$49</f>
         <v>101.20000000000002</v>
       </c>
       <c r="G54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*G$49</f>
         <v>119.60000000000001</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*H$49</f>
         <v>138.00000000000003</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*I$49</f>
         <v>156.4</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="4"/>
+        <f>$C30/100*Light_units_generated_standard*J$49</f>
         <v>174.8</v>
       </c>
     </row>
@@ -1548,39 +1766,39 @@
         <v>5</v>
       </c>
       <c r="B55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*B$49</f>
         <v>30</v>
       </c>
       <c r="C55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*C$49</f>
         <v>50</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*D$49</f>
         <v>70</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*E$49</f>
         <v>90</v>
       </c>
       <c r="F55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*F$49</f>
         <v>110</v>
       </c>
       <c r="G55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*G$49</f>
         <v>130</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*H$49</f>
         <v>150</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*I$49</f>
         <v>170</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="4"/>
+        <f>$C31/100*Light_units_generated_standard*J$49</f>
         <v>190</v>
       </c>
     </row>
@@ -1643,35 +1861,35 @@
         <v>0</v>
       </c>
       <c r="B60" s="2">
-        <f>(B$59*$C26-(B$59-2)*$C27)/100*$B$47</f>
+        <f>(B$59*$C26-(B$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-3.4000000000000004</v>
       </c>
       <c r="C60" s="2">
-        <f t="shared" ref="C60:I60" si="5">(C$59*$C26-(C$59-2)*$C27)/100*$B$47</f>
+        <f>(C$59*$C26-(C$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-10.199999999999999</v>
       </c>
       <c r="D60" s="2">
-        <f t="shared" si="5"/>
+        <f>(D$59*$C26-(D$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-17</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="5"/>
+        <f>(E$59*$C26-(E$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-23.799999999999997</v>
       </c>
       <c r="F60" s="2">
-        <f t="shared" si="5"/>
+        <f>(F$59*$C26-(F$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-30.6</v>
       </c>
       <c r="G60" s="2">
-        <f t="shared" si="5"/>
+        <f>(G$59*$C26-(G$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-37.400000000000006</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" si="5"/>
+        <f>(H$59*$C26-(H$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-44.2</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="5"/>
+        <f>(I$59*$C26-(I$59-2)*$C27)/100*Light_units_generated_standard</f>
         <v>-51</v>
       </c>
       <c r="J60" s="2"/>
@@ -1681,35 +1899,35 @@
         <v>1</v>
       </c>
       <c r="B61" s="2">
-        <f t="shared" ref="B61:I64" si="6">(B$59*$C27-(B$59-2)*$C28)/100*$B$47</f>
+        <f>(B$59*$C27-(B$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>11.200000000000001</v>
       </c>
       <c r="C61" s="2">
-        <f t="shared" si="6"/>
+        <f>(C$59*$C27-(C$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>9.6</v>
       </c>
       <c r="D61" s="2">
-        <f t="shared" si="6"/>
+        <f>(D$59*$C27-(D$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>8</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="6"/>
+        <f>(E$59*$C27-(E$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>6.4</v>
       </c>
       <c r="F61" s="2">
-        <f t="shared" si="6"/>
+        <f>(F$59*$C27-(F$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>4.8</v>
       </c>
       <c r="G61" s="2">
-        <f t="shared" si="6"/>
+        <f>(G$59*$C27-(G$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>3.2</v>
       </c>
       <c r="H61" s="2">
-        <f t="shared" si="6"/>
+        <f>(H$59*$C27-(H$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>1.6</v>
       </c>
       <c r="I61" s="2">
-        <f t="shared" si="6"/>
+        <f>(I$59*$C27-(I$59-2)*$C28)/100*Light_units_generated_standard</f>
         <v>0</v>
       </c>
       <c r="J61" s="2"/>
@@ -1719,35 +1937,35 @@
         <v>2</v>
       </c>
       <c r="B62" s="2">
-        <f t="shared" si="6"/>
+        <f>(B$59*$C28-(B$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>12.8</v>
       </c>
       <c r="C62" s="2">
-        <f t="shared" si="6"/>
+        <f>(C$59*$C28-(C$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>11.200000000000001</v>
       </c>
       <c r="D62" s="2">
-        <f t="shared" si="6"/>
+        <f>(D$59*$C28-(D$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>9.6</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="6"/>
+        <f>(E$59*$C28-(E$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>8</v>
       </c>
       <c r="F62" s="2">
-        <f t="shared" si="6"/>
+        <f>(F$59*$C28-(F$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>6.4</v>
       </c>
       <c r="G62" s="2">
-        <f t="shared" si="6"/>
+        <f>(G$59*$C28-(G$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>4.8</v>
       </c>
       <c r="H62" s="2">
-        <f t="shared" si="6"/>
+        <f>(H$59*$C28-(H$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>3.2</v>
       </c>
       <c r="I62" s="2">
-        <f t="shared" si="6"/>
+        <f>(I$59*$C28-(I$59-2)*$C29)/100*Light_units_generated_standard</f>
         <v>1.6</v>
       </c>
       <c r="J62" s="2"/>
@@ -1757,35 +1975,35 @@
         <v>3</v>
       </c>
       <c r="B63" s="2">
-        <f t="shared" si="6"/>
+        <f>(B$59*$C29-(B$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>14.399999999999999</v>
       </c>
       <c r="C63" s="2">
-        <f t="shared" si="6"/>
+        <f>(C$59*$C29-(C$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>12.8</v>
       </c>
       <c r="D63" s="2">
-        <f t="shared" si="6"/>
+        <f>(D$59*$C29-(D$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>11.200000000000001</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="6"/>
+        <f>(E$59*$C29-(E$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>9.6</v>
       </c>
       <c r="F63" s="2">
-        <f t="shared" si="6"/>
+        <f>(F$59*$C29-(F$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>8</v>
       </c>
       <c r="G63" s="2">
-        <f t="shared" si="6"/>
+        <f>(G$59*$C29-(G$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>6.4</v>
       </c>
       <c r="H63" s="2">
-        <f t="shared" si="6"/>
+        <f>(H$59*$C29-(H$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>4.8</v>
       </c>
       <c r="I63" s="2">
-        <f t="shared" si="6"/>
+        <f>(I$59*$C29-(I$59-2)*$C30)/100*Light_units_generated_standard</f>
         <v>3.2</v>
       </c>
       <c r="J63" s="2"/>
@@ -1795,40 +2013,40 @@
         <v>4</v>
       </c>
       <c r="B64" s="2">
-        <f t="shared" si="6"/>
+        <f>(B$59*$C30-(B$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>16</v>
       </c>
       <c r="C64" s="2">
-        <f t="shared" si="6"/>
+        <f>(C$59*$C30-(C$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>14.399999999999999</v>
       </c>
       <c r="D64" s="2">
-        <f t="shared" si="6"/>
+        <f>(D$59*$C30-(D$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>12.8</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="6"/>
+        <f>(E$59*$C30-(E$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>11.200000000000001</v>
       </c>
       <c r="F64" s="2">
-        <f t="shared" si="6"/>
+        <f>(F$59*$C30-(F$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>9.6</v>
       </c>
       <c r="G64" s="2">
-        <f t="shared" si="6"/>
+        <f>(G$59*$C30-(G$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>8</v>
       </c>
       <c r="H64" s="2">
-        <f t="shared" si="6"/>
+        <f>(H$59*$C30-(H$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>6.4</v>
       </c>
       <c r="I64" s="2">
-        <f t="shared" si="6"/>
+        <f>(I$59*$C30-(I$59-2)*$C31)/100*Light_units_generated_standard</f>
         <v>4.8</v>
       </c>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -1839,20 +2057,29 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>35</v>
-      </c>
-      <c r="K67" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C67" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67">
+        <v>84</v>
+      </c>
+      <c r="E67" t="s">
+        <v>39</v>
+      </c>
+      <c r="F67">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -1883,602 +2110,695 @@
       <c r="J68">
         <v>19</v>
       </c>
-      <c r="K68">
-        <v>3</v>
-      </c>
-      <c r="L68">
-        <v>5</v>
-      </c>
-      <c r="M68">
-        <v>7</v>
-      </c>
-      <c r="N68">
-        <v>9</v>
-      </c>
-      <c r="O68">
-        <v>11</v>
-      </c>
-      <c r="P68">
-        <v>13</v>
-      </c>
-      <c r="Q68">
-        <v>15</v>
-      </c>
-      <c r="R68">
-        <v>17</v>
-      </c>
-      <c r="S68">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4</v>
       </c>
       <c r="B69">
-        <f>IF(B$68&lt;2*$A69,$C$29/100*B$68*$B$47-($A69*B$68/$B$77)^$B$78,"N/A")</f>
-        <v>9.094824156799806</v>
+        <f>IF(B$68&lt;2*$A69,Set_foilage_density/100*B$68*Set_light_input-($A69*B$68/divider)^exponent,"N/A")</f>
+        <v>14.133739060297231</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69:J69" si="7">IF(C$68&lt;2*$A69,$C$29/100*C$68*$B$47-($A69*C$68/$B$77)^$B$78,"N/A")</f>
-        <v>16.825114763331111</v>
+        <f>IF(C$68&lt;2*$A69,Set_foilage_density/100*C$68*Set_light_input-($A69*C$68/divider)^exponent,"N/A")</f>
+        <v>25.223145943577325</v>
       </c>
       <c r="D69">
-        <f t="shared" si="7"/>
-        <v>25.012709271425585</v>
+        <f>IF(D$68&lt;2*$A69,Set_foilage_density/100*D$68*Set_light_input-($A69*D$68/divider)^exponent,"N/A")</f>
+        <v>36.76982588570651</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E$68&lt;2*$A69,Set_foilage_density/100*E$68*Set_light_input-($A69*E$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(F$68&lt;2*$A69,Set_foilage_density/100*F$68*Set_light_input-($A69*F$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(G$68&lt;2*$A69,Set_foilage_density/100*G$68*Set_light_input-($A69*G$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H$68&lt;2*$A69,Set_foilage_density/100*H$68*Set_light_input-($A69*H$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(I$68&lt;2*$A69,Set_foilage_density/100*I$68*Set_light_input-($A69*I$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="7"/>
-        <v>N/A</v>
-      </c>
-      <c r="K69">
-        <f>IF(K$68&lt;2*$A69,$C$31/100*K$68*$B$47-($A69*K$68/$B$77)^$B$78,"N/A")</f>
-        <v>13.894824156799807</v>
-      </c>
-      <c r="L69">
-        <f t="shared" ref="L69:S69" si="8">IF(L$68&lt;2*$A69,$C$31/100*L$68*$B$47-($A69*L$68/$B$77)^$B$78,"N/A")</f>
-        <v>24.825114763331111</v>
-      </c>
-      <c r="M69">
-        <f t="shared" si="8"/>
-        <v>36.212709271425588</v>
-      </c>
-      <c r="N69" t="str">
-        <f t="shared" si="8"/>
-        <v>N/A</v>
-      </c>
-      <c r="O69" t="str">
-        <f t="shared" si="8"/>
-        <v>N/A</v>
-      </c>
-      <c r="P69" t="str">
-        <f t="shared" si="8"/>
-        <v>N/A</v>
-      </c>
-      <c r="Q69" t="str">
-        <f t="shared" si="8"/>
-        <v>N/A</v>
-      </c>
-      <c r="R69" t="str">
-        <f t="shared" si="8"/>
-        <v>N/A</v>
-      </c>
-      <c r="S69" t="str">
-        <f t="shared" si="8"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(J$68&lt;2*$A69,Set_foilage_density/100*J$68*Set_light_input-($A69*J$68/divider)^exponent,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5</v>
       </c>
       <c r="B70">
-        <f t="shared" ref="B70:J75" si="9">IF(B$68&lt;2*$A70,$C$29/100*B$68*$B$47-($A70*B$68/$B$77)^$B$78,"N/A")</f>
-        <v>5.6245739558420276</v>
+        <f>IF(B$68&lt;2*$A70,Set_foilage_density/100*B$68*Set_light_input-($A70*B$68/divider)^exponent,"N/A")</f>
+        <v>10.663162440087536</v>
       </c>
       <c r="C70">
-        <f t="shared" si="9"/>
-        <v>11.400576006213168</v>
+        <f>IF(C$68&lt;2*$A70,Set_foilage_density/100*C$68*Set_light_input-($A70*C$68/divider)^exponent,"N/A")</f>
+        <v>19.798038192885137</v>
       </c>
       <c r="D70">
-        <f t="shared" si="9"/>
-        <v>17.732419159588105</v>
+        <f>IF(D$68&lt;2*$A70,Set_foilage_density/100*D$68*Set_light_input-($A70*D$68/divider)^exponent,"N/A")</f>
+        <v>29.488720189424008</v>
       </c>
       <c r="E70">
-        <f t="shared" si="9"/>
-        <v>24.438455662388158</v>
+        <f>IF(E$68&lt;2*$A70,Set_foilage_density/100*E$68*Set_light_input-($A70*E$68/divider)^exponent,"N/A")</f>
+        <v>39.553574924127119</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(F$68&lt;2*$A70,Set_foilage_density/100*F$68*Set_light_input-($A70*F$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(G$68&lt;2*$A70,Set_foilage_density/100*G$68*Set_light_input-($A70*G$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(H$68&lt;2*$A70,Set_foilage_density/100*H$68*Set_light_input-($A70*H$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(I$68&lt;2*$A70,Set_foilage_density/100*I$68*Set_light_input-($A70*I$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="9"/>
-        <v>N/A</v>
-      </c>
-      <c r="K70">
-        <f t="shared" ref="K70:S75" si="10">IF(K$68&lt;2*$A70,$C$31/100*K$68*$B$47-($A70*K$68/$B$77)^$B$78,"N/A")</f>
-        <v>10.424573955842028</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="10"/>
-        <v>19.400576006213168</v>
-      </c>
-      <c r="M70">
-        <f t="shared" si="10"/>
-        <v>28.932419159588108</v>
-      </c>
-      <c r="N70">
-        <f t="shared" si="10"/>
-        <v>38.838455662388164</v>
-      </c>
-      <c r="O70" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="P70" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="Q70" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="R70" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="S70" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(J$68&lt;2*$A70,Set_foilage_density/100*J$68*Set_light_input-($A70*J$68/divider)^exponent,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>6</v>
       </c>
       <c r="B71">
-        <f t="shared" si="9"/>
-        <v>2.2409695533584468</v>
+        <f>IF(B$68&lt;2*$A71,Set_foilage_density/100*B$68*Set_light_input-($A71*B$68/divider)^exponent,"N/A")</f>
+        <v>7.2792253112845628</v>
       </c>
       <c r="C71">
-        <f t="shared" si="9"/>
-        <v>6.1114780573213778</v>
+        <f>IF(C$68&lt;2*$A71,Set_foilage_density/100*C$68*Set_light_input-($A71*C$68/divider)^exponent,"N/A")</f>
+        <v>14.508362858123391</v>
       </c>
       <c r="D71">
-        <f t="shared" si="9"/>
-        <v>10.633904572088881</v>
+        <f>IF(D$68&lt;2*$A71,Set_foilage_density/100*D$68*Set_light_input-($A71*D$68/divider)^exponent,"N/A")</f>
+        <v>22.389380050695053</v>
       </c>
       <c r="E71">
-        <f t="shared" si="9"/>
-        <v>15.595203604011381</v>
+        <f>IF(E$68&lt;2*$A71,Set_foilage_density/100*E$68*Set_light_input-($A71*E$68/divider)^exponent,"N/A")</f>
+        <v>30.709247282725549</v>
       </c>
       <c r="F71">
-        <f t="shared" si="9"/>
-        <v>20.885032174381934</v>
+        <f>IF(F$68&lt;2*$A71,Set_foilage_density/100*F$68*Set_light_input-($A71*F$68/divider)^exponent,"N/A")</f>
+        <v>39.357629041480976</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(G$68&lt;2*$A71,Set_foilage_density/100*G$68*Set_light_input-($A71*G$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(H$68&lt;2*$A71,Set_foilage_density/100*H$68*Set_light_input-($A71*H$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(I$68&lt;2*$A71,Set_foilage_density/100*I$68*Set_light_input-($A71*I$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" si="9"/>
-        <v>N/A</v>
-      </c>
-      <c r="K71">
-        <f t="shared" si="10"/>
-        <v>7.0409695533584475</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="10"/>
-        <v>14.111478057321378</v>
-      </c>
-      <c r="M71">
-        <f t="shared" si="10"/>
-        <v>21.833904572088883</v>
-      </c>
-      <c r="N71">
-        <f t="shared" si="10"/>
-        <v>29.995203604011387</v>
-      </c>
-      <c r="O71">
-        <f t="shared" si="10"/>
-        <v>38.485032174381928</v>
-      </c>
-      <c r="P71" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="Q71" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="R71" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="S71" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(J$68&lt;2*$A71,Set_foilage_density/100*J$68*Set_light_input-($A71*J$68/divider)^exponent,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>7</v>
       </c>
       <c r="B72">
-        <f t="shared" si="9"/>
-        <v>-1.0722393636297092</v>
+        <f>IF(B$68&lt;2*$A72,Set_foilage_density/100*B$68*Set_light_input-($A72*B$68/divider)^exponent,"N/A")</f>
+        <v>3.9656788209434417</v>
       </c>
       <c r="C72">
-        <f t="shared" si="9"/>
-        <v>0.9324191595881075</v>
+        <f>IF(C$68&lt;2*$A72,Set_foilage_density/100*C$68*Set_light_input-($A72*C$68/divider)^exponent,"N/A")</f>
+        <v>9.3287201894240113</v>
       </c>
       <c r="D72">
-        <f t="shared" si="9"/>
-        <v>3.6830737328187411</v>
+        <f>IF(D$68&lt;2*$A72,Set_foilage_density/100*D$68*Set_light_input-($A72*D$68/divider)^exponent,"N/A")</f>
+        <v>15.437716144118653</v>
       </c>
       <c r="E72">
-        <f t="shared" si="9"/>
-        <v>6.9359343485742784</v>
+        <f>IF(E$68&lt;2*$A72,Set_foilage_density/100*E$68*Set_light_input-($A72*E$68/divider)^exponent,"N/A")</f>
+        <v>22.048894060985958</v>
       </c>
       <c r="F72">
-        <f t="shared" si="9"/>
-        <v>10.564734475024153</v>
+        <f>IF(F$68&lt;2*$A72,Set_foilage_density/100*F$68*Set_light_input-($A72*F$68/divider)^exponent,"N/A")</f>
+        <v>29.035995538977545</v>
       </c>
       <c r="G72">
-        <f t="shared" si="9"/>
-        <v>14.49246868660596</v>
+        <f>IF(G$68&lt;2*$A72,Set_foilage_density/100*G$68*Set_light_input-($A72*G$68/divider)^exponent,"N/A")</f>
+        <v>36.322019720214584</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(H$68&lt;2*$A72,Set_foilage_density/100*H$68*Set_light_input-($A72*H$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(I$68&lt;2*$A72,Set_foilage_density/100*I$68*Set_light_input-($A72*I$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" si="9"/>
-        <v>N/A</v>
-      </c>
-      <c r="K72">
-        <f t="shared" si="10"/>
-        <v>3.7277606363702915</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="10"/>
-        <v>8.9324191595881075</v>
-      </c>
-      <c r="M72">
-        <f t="shared" si="10"/>
-        <v>14.883073732818744</v>
-      </c>
-      <c r="N72">
-        <f t="shared" si="10"/>
-        <v>21.335934348574284</v>
-      </c>
-      <c r="O72">
-        <f t="shared" si="10"/>
-        <v>28.164734475024147</v>
-      </c>
-      <c r="P72">
-        <f t="shared" si="10"/>
-        <v>35.292468686605957</v>
-      </c>
-      <c r="Q72" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="R72" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="S72" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(J$68&lt;2*$A72,Set_foilage_density/100*J$68*Set_light_input-($A72*J$68/divider)^exponent,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>8</v>
       </c>
       <c r="B73">
-        <f t="shared" si="9"/>
-        <v>-4.3263538752905824</v>
+        <f>IF(B$68&lt;2*$A73,Set_foilage_density/100*B$68*Set_light_input-($A73*B$68/divider)^exponent,"N/A")</f>
+        <v>0.71122286267887347</v>
       </c>
       <c r="C73">
-        <f t="shared" si="9"/>
-        <v>-4.1542660263193412</v>
+        <f>IF(C$68&lt;2*$A73,Set_foilage_density/100*C$68*Set_light_input-($A73*C$68/divider)^exponent,"N/A")</f>
+        <v>4.2414461783403894</v>
       </c>
       <c r="D73">
-        <f t="shared" si="9"/>
-        <v>-3.1437820643490824</v>
+        <f>IF(D$68&lt;2*$A73,Set_foilage_density/100*D$68*Set_light_input-($A73*D$68/divider)^exponent,"N/A")</f>
+        <v>8.6100213806505721</v>
       </c>
       <c r="E73">
-        <f t="shared" si="9"/>
-        <v>-1.5688881514545301</v>
+        <f>IF(E$68&lt;2*$A73,Set_foilage_density/100*E$68*Set_light_input-($A73*E$68/divider)^exponent,"N/A")</f>
+        <v>13.542981068570242</v>
       </c>
       <c r="F73">
-        <f t="shared" si="9"/>
-        <v>0.42850963995741154</v>
+        <f>IF(F$68&lt;2*$A73,Set_foilage_density/100*F$68*Set_light_input-($A73*F$68/divider)^exponent,"N/A")</f>
+        <v>18.898427905880382</v>
       </c>
       <c r="G73">
-        <f t="shared" si="9"/>
-        <v>2.7618678898905102</v>
+        <f>IF(G$68&lt;2*$A73,Set_foilage_density/100*G$68*Set_light_input-($A73*G$68/divider)^exponent,"N/A")</f>
+        <v>24.589823361054428</v>
       </c>
       <c r="H73">
-        <f t="shared" si="9"/>
-        <v>5.3730709947855786</v>
+        <f>IF(H$68&lt;2*$A73,Set_foilage_density/100*H$68*Set_light_input-($A73*H$68/divider)^exponent,"N/A")</f>
+        <v>30.559054878056912</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="9"/>
+        <f>IF(I$68&lt;2*$A73,Set_foilage_density/100*I$68*Set_light_input-($A73*I$68/divider)^exponent,"N/A")</f>
         <v>N/A</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="9"/>
-        <v>N/A</v>
-      </c>
-      <c r="K73">
-        <f t="shared" si="10"/>
-        <v>0.47364612470941836</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="10"/>
-        <v>3.8457339736806588</v>
-      </c>
-      <c r="M73">
-        <f t="shared" si="10"/>
-        <v>8.0562179356509205</v>
-      </c>
-      <c r="N73">
-        <f t="shared" si="10"/>
-        <v>12.831111848545476</v>
-      </c>
-      <c r="O73">
-        <f t="shared" si="10"/>
-        <v>18.028509639957406</v>
-      </c>
-      <c r="P73">
-        <f t="shared" si="10"/>
-        <v>23.561867889890507</v>
-      </c>
-      <c r="Q73">
-        <f t="shared" si="10"/>
-        <v>29.373070994785579</v>
-      </c>
-      <c r="R73" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-      <c r="S73" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(J$68&lt;2*$A73,Set_foilage_density/100*J$68*Set_light_input-($A73*J$68/divider)^exponent,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9</v>
       </c>
       <c r="B74">
-        <f t="shared" si="9"/>
-        <v>-7.5296692803493563</v>
+        <f>IF(B$68&lt;2*$A74,Set_foilage_density/100*B$68*Set_light_input-($A74*B$68/divider)^exponent,"N/A")</f>
+        <v>-2.492437173322287</v>
       </c>
       <c r="C74">
-        <f t="shared" si="9"/>
-        <v>-9.1615443376118364</v>
+        <f>IF(C$68&lt;2*$A74,Set_foilage_density/100*C$68*Set_light_input-($A74*C$68/divider)^exponent,"N/A")</f>
+        <v>-0.76642507587287412</v>
       </c>
       <c r="D74">
-        <f t="shared" si="9"/>
-        <v>-9.8640656514257188</v>
+        <f>IF(D$68&lt;2*$A74,Set_foilage_density/100*D$68*Set_light_input-($A74*D$68/divider)^exponent,"N/A")</f>
+        <v>1.8888940609859617</v>
       </c>
       <c r="E74">
-        <f t="shared" si="9"/>
-        <v>-9.9409441544031125</v>
+        <f>IF(E$68&lt;2*$A74,Set_foilage_density/100*E$68*Set_light_input-($A74*E$68/divider)^exponent,"N/A")</f>
+        <v>5.1698293427634212</v>
       </c>
       <c r="F74">
-        <f t="shared" si="9"/>
-        <v>-9.5494813148651758</v>
+        <f>IF(F$68&lt;2*$A74,Set_foilage_density/100*F$68*Set_light_input-($A74*F$68/divider)^exponent,"N/A")</f>
+        <v>8.9190885923653695</v>
       </c>
       <c r="G74">
-        <f t="shared" si="9"/>
-        <v>-8.7856096521749834</v>
+        <f>IF(G$68&lt;2*$A74,Set_foilage_density/100*G$68*Set_light_input-($A74*G$68/divider)^exponent,"N/A")</f>
+        <v>13.040744469723336</v>
       </c>
       <c r="H74">
-        <f t="shared" si="9"/>
-        <v>-7.7137497342277754</v>
+        <f>IF(H$68&lt;2*$A74,Set_foilage_density/100*H$68*Set_light_input-($A74*H$68/divider)^exponent,"N/A")</f>
+        <v>17.470379624245055</v>
       </c>
       <c r="I74">
-        <f t="shared" si="9"/>
-        <v>-6.3800303727618655</v>
+        <f>IF(I$68&lt;2*$A74,Set_foilage_density/100*I$68*Set_light_input-($A74*I$68/divider)^exponent,"N/A")</f>
+        <v>22.161867392269414</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" si="9"/>
-        <v>N/A</v>
-      </c>
-      <c r="K74">
-        <f t="shared" si="10"/>
-        <v>-2.7296692803493556</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="10"/>
-        <v>-1.1615443376118364</v>
-      </c>
-      <c r="M74">
-        <f t="shared" si="10"/>
-        <v>1.3359343485742841</v>
-      </c>
-      <c r="N74">
-        <f t="shared" si="10"/>
-        <v>4.4590558455968932</v>
-      </c>
-      <c r="O74">
-        <f t="shared" si="10"/>
-        <v>8.0505186851348185</v>
-      </c>
-      <c r="P74">
-        <f t="shared" si="10"/>
-        <v>12.014390347825014</v>
-      </c>
-      <c r="Q74">
-        <f t="shared" si="10"/>
-        <v>16.286250265772225</v>
-      </c>
-      <c r="R74">
-        <f t="shared" si="10"/>
-        <v>20.819969627238152</v>
-      </c>
-      <c r="S74" t="str">
-        <f t="shared" si="10"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(J$68&lt;2*$A74,Set_foilage_density/100*J$68*Set_light_input-($A74*J$68/divider)^exponent,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>10</v>
       </c>
       <c r="B75">
-        <f t="shared" si="9"/>
-        <v>-10.688521942678623</v>
+        <f>IF(B$68&lt;2*$A75,Set_foilage_density/100*B$68*Set_light_input-($A75*B$68/divider)^exponent,"N/A")</f>
+        <v>-5.6516371418766127</v>
       </c>
       <c r="C75">
-        <f t="shared" si="9"/>
-        <v>-14.099320492801198</v>
+        <f>IF(C$68&lt;2*$A75,Set_foilage_density/100*C$68*Set_light_input-($A75*C$68/divider)^exponent,"N/A")</f>
+        <v>-5.7047976032470658</v>
       </c>
       <c r="D75">
-        <f t="shared" si="9"/>
-        <v>-16.491070181519845</v>
+        <f>IF(D$68&lt;2*$A75,Set_foilage_density/100*D$68*Set_light_input-($A75*D$68/divider)^exponent,"N/A")</f>
+        <v>-4.7389581387866855</v>
       </c>
       <c r="E75">
-        <f t="shared" si="9"/>
-        <v>-18.196794125442409</v>
+        <f>IF(E$68&lt;2*$A75,Set_foilage_density/100*E$68*Set_light_input-($A75*E$68/divider)^exponent,"N/A")</f>
+        <v>-3.0871206368255741</v>
       </c>
       <c r="F75">
-        <f t="shared" si="9"/>
-        <v>-19.38897549722482</v>
+        <f>IF(F$68&lt;2*$A75,Set_foilage_density/100*F$68*Set_light_input-($A75*F$68/divider)^exponent,"N/A")</f>
+        <v>-0.92175846730008004</v>
       </c>
       <c r="G75">
-        <f t="shared" si="9"/>
-        <v>-20.172805592773031</v>
+        <f>IF(G$68&lt;2*$A75,Set_foilage_density/100*G$68*Set_light_input-($A75*G$68/divider)^exponent,"N/A")</f>
+        <v>1.651942518107262</v>
       </c>
       <c r="H75">
-        <f t="shared" si="9"/>
-        <v>-20.618922429987009</v>
+        <f>IF(H$68&lt;2*$A75,Set_foilage_density/100*H$68*Set_light_input-($A75*H$68/divider)^exponent,"N/A")</f>
+        <v>4.5633476715435108</v>
       </c>
       <c r="I75">
-        <f t="shared" si="9"/>
-        <v>-20.777906870471895</v>
+        <f>IF(I$68&lt;2*$A75,Set_foilage_density/100*I$68*Set_light_input-($A75*I$68/divider)^exponent,"N/A")</f>
+        <v>7.7618783738264199</v>
       </c>
       <c r="J75">
-        <f t="shared" si="9"/>
-        <v>-20.687686152213757</v>
-      </c>
-      <c r="K75">
-        <f t="shared" si="10"/>
-        <v>-5.8885219426786222</v>
-      </c>
-      <c r="L75">
-        <f t="shared" si="10"/>
-        <v>-6.0993204928011977</v>
-      </c>
-      <c r="M75">
-        <f t="shared" si="10"/>
-        <v>-5.2910701815198422</v>
-      </c>
-      <c r="N75">
-        <f t="shared" si="10"/>
-        <v>-3.7967941254424034</v>
-      </c>
-      <c r="O75">
-        <f t="shared" si="10"/>
-        <v>-1.7889754972248255</v>
-      </c>
-      <c r="P75">
-        <f t="shared" si="10"/>
-        <v>0.62719440722696618</v>
-      </c>
-      <c r="Q75">
-        <f t="shared" si="10"/>
-        <v>3.3810775700129909</v>
-      </c>
-      <c r="R75">
-        <f t="shared" si="10"/>
-        <v>6.4220931295281218</v>
-      </c>
-      <c r="S75">
-        <f t="shared" si="10"/>
-        <v>9.7123138477862483</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(J$68&lt;2*$A75,Set_foilage_density/100*J$68*Set_light_input-($A75*J$68/divider)^exponent,"N/A")</f>
+        <v>11.209608958440725</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B77">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>38</v>
+        <f>ROUND(LOG(190)/(LOG(190)-LOG(B76))*0.99,4)</f>
+        <v>0.87450000000000006</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>190</v>
       </c>
       <c r="B78">
-        <f>LOG(190)/(LOG(190)-LOG(B77))*0.99</f>
-        <v>0.87447880043187665</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
-        <v>190</v>
-      </c>
-      <c r="B79">
-        <f>(190/B77)^B78</f>
-        <v>180.28768615221375</v>
+        <f>(190/B76)^B77</f>
+        <v>180.31039104155926</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82">
+        <f>F82</f>
+        <v>50</v>
+      </c>
+      <c r="E82" t="s">
+        <v>75</v>
+      </c>
+      <c r="F82">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83">
+        <f>$F$82*$F$83*A83/100</f>
+        <v>2.5</v>
+      </c>
+      <c r="C83">
+        <f>F$82*(1-F$83/100)^A83</f>
+        <v>47.5</v>
+      </c>
+      <c r="D83">
+        <f>C82*F$83/8</f>
+        <v>31.25</v>
+      </c>
+      <c r="E83" t="s">
+        <v>76</v>
+      </c>
+      <c r="F83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="B84">
+        <f>$F$82*$F$83*A84/100</f>
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <f t="shared" ref="C84:C102" si="3">F$82*(1-F$83/100)^A84</f>
+        <v>45.125</v>
+      </c>
+      <c r="D84">
+        <f t="shared" ref="D84:D102" si="4">C83*F$83/8</f>
+        <v>29.6875</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <f>$F$82*$F$83*A85/100</f>
+        <v>7.5</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="3"/>
+        <v>42.868749999999991</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="4"/>
+        <v>28.203125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>4</v>
+      </c>
+      <c r="B86">
+        <f>$F$82*$F$83*A86/100</f>
+        <v>10</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="3"/>
+        <v>40.725312500000001</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="4"/>
+        <v>26.792968749999993</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <f>$F$82*$F$83*A87/100</f>
+        <v>12.5</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="3"/>
+        <v>38.689046875000003</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="4"/>
+        <v>25.453320312500001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>6</v>
+      </c>
+      <c r="B88">
+        <f>$F$82*$F$83*A88/100</f>
+        <v>15</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="3"/>
+        <v>36.754594531249992</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="4"/>
+        <v>24.180654296875002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>7</v>
+      </c>
+      <c r="B89">
+        <f>$F$82*$F$83*A89/100</f>
+        <v>17.5</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="3"/>
+        <v>34.916864804687499</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="4"/>
+        <v>22.971621582031247</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>8</v>
+      </c>
+      <c r="B90">
+        <f>$F$82*$F$83*A90/100</f>
+        <v>20</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="3"/>
+        <v>33.17102156445312</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="4"/>
+        <v>21.823040502929686</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>9</v>
+      </c>
+      <c r="B91">
+        <f>$F$82*$F$83*A91/100</f>
+        <v>22.5</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="3"/>
+        <v>31.512470486230466</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="4"/>
+        <v>20.731888477783201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>10</v>
+      </c>
+      <c r="B92">
+        <f>$F$82*$F$83*A92/100</f>
+        <v>25</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="3"/>
+        <v>29.936846961918945</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="4"/>
+        <v>19.695294053894042</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>11</v>
+      </c>
+      <c r="B93">
+        <f>$F$82*$F$83*A93/100</f>
+        <v>27.5</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="3"/>
+        <v>28.440004613822996</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="4"/>
+        <v>18.710529351199341</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>12</v>
+      </c>
+      <c r="B94">
+        <f>$F$82*$F$83*A94/100</f>
+        <v>30</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="3"/>
+        <v>27.018004383131846</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="4"/>
+        <v>17.775002883639374</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>13</v>
+      </c>
+      <c r="B95">
+        <f>$F$82*$F$83*A95/100</f>
+        <v>32.5</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="3"/>
+        <v>25.667104163975253</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="4"/>
+        <v>16.886252739457404</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>14</v>
+      </c>
+      <c r="B96">
+        <f>$F$82*$F$83*A96/100</f>
+        <v>35</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="3"/>
+        <v>24.38374895577649</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="4"/>
+        <v>16.041940102484531</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>15</v>
+      </c>
+      <c r="B97">
+        <f>$F$82*$F$83*A97/100</f>
+        <v>37.5</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="3"/>
+        <v>23.164561507987667</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="4"/>
+        <v>15.239843097360307</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>16</v>
+      </c>
+      <c r="B98">
+        <f>$F$82*$F$83*A98/100</f>
+        <v>40</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="3"/>
+        <v>22.006333432588281</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="4"/>
+        <v>14.477850942492292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>17</v>
+      </c>
+      <c r="B99">
+        <f>$F$82*$F$83*A99/100</f>
+        <v>42.5</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="3"/>
+        <v>20.906016760958867</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="4"/>
+        <v>13.753958395367675</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>18</v>
+      </c>
+      <c r="B100">
+        <f>$F$82*$F$83*A100/100</f>
+        <v>45</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="3"/>
+        <v>19.860715922910924</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="4"/>
+        <v>13.066260475599291</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>19</v>
+      </c>
+      <c r="B101">
+        <f>$F$82*$F$83*A101/100</f>
+        <v>47.5</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="3"/>
+        <v>18.867680126765375</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="4"/>
+        <v>12.412947451819328</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>20</v>
+      </c>
+      <c r="B102">
+        <f>$F$82*$F$83*A102/100</f>
+        <v>50</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="3"/>
+        <v>17.924296120427108</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="4"/>
+        <v>11.79230007922836</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>77</v>
+      </c>
+      <c r="B105" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B60:I64">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2490,25 +2810,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69:J75">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69:S75">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69:S75">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69:S75">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F67">
+      <formula1>"8,10,12"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D67">
+      <formula1>C26:C31</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2517,12 +2855,149 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2530,12 +3005,462 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>80</v>
+      </c>
+      <c r="G72" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <v>34</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="G73" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>68</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="B75">
+        <v>76</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>84</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>4</v>
+      </c>
+      <c r="B77">
+        <v>92</v>
+      </c>
+      <c r="C77">
+        <v>5</v>
+      </c>
+      <c r="D77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tweaked water intake in game design a lot.
</commit_message>
<xml_diff>
--- a/game_design/TreeWars_balancing.xlsx
+++ b/game_design/TreeWars_balancing.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="153">
   <si>
     <t>Basics</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>Costs 10 Hazard points to activate</t>
+  </si>
+  <si>
+    <t>This chance is divided by 2 for every tree the storm has already hit</t>
   </si>
 </sst>
 </file>
@@ -6929,8 +6932,8 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7323,7 +7326,7 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>